<commit_message>
game count at 504
</commit_message>
<xml_diff>
--- a/code/video_links.xlsx
+++ b/code/video_links.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="749">
   <si>
     <t>Team 1</t>
   </si>
@@ -1875,6 +1875,405 @@
   </si>
   <si>
     <t xml:space="preserve"> _RkY862mvZg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/25/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vI_WBjrr8kw</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers</t>
+  </si>
+  <si>
+    <t>Mi3lZ3AArPY</t>
+  </si>
+  <si>
+    <t>UQ6xvxy_aBU</t>
+  </si>
+  <si>
+    <t>7EtCV1vxBmQ</t>
+  </si>
+  <si>
+    <t>pYn4ugyoaeU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/21/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JzZ5EhUvhsk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33P9xYweBro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OwtrqtLw4EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/20/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0lcPPKDXo-M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indina Pacers </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> agKS3iH0PGU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/19/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e5LL5lwIwhA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 46cjktgpPew</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/18/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jilFle0ibQE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4uVYl1GrXL4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7hlI3YyvnNw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/17/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ujqX6nE69sg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x-wb4LpIZKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7zh3o3QKVLQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/16/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IIVrZGnW76w</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5tMRHg1te-Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AYbhlGF2Xcg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xHTHkLcZMoE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/15/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89_zzpD-OlU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lruiE83ZqmA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IWVVmit8d1w</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> J9yz2UETuTw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> daUzMnrdWhQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/14/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dh1w76HrgRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FG1RpcR1-a0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UtGr3wOKb7c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _fgHRZe0Huc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/13/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zhKHmQ1Sq7Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1UOA_zL8qeU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WxJVJP0-Vl0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5svSmUOoPHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vMDsGBeHXJ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oRaeu2EhU38</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jCbjUFIgPfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/11/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -_HJvzYEflc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gWoCc79-aaQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/10/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OgLFo49nyXw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FNNPdHhzA64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MoiDPRbyDME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> aOxzhkjjB1Q</t>
+  </si>
+  <si>
+    <t>LaQdT_hCpZo</t>
+  </si>
+  <si>
+    <t>zg7aAUadp0Y</t>
+  </si>
+  <si>
+    <t>8Qwjb6ZVl8E</t>
+  </si>
+  <si>
+    <t>nDK539R1Y2Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/8/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v2jJPfN007s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0yOTPaT_r4g</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> QpAzD5iTsVg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> evmcPgG9dzg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/7/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nyVJOz4bIvY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C_7fgm89BXY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cif_Rx60j0w</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kg_USJHAgPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/6/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rviTVRqIxVY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ydKAYHe2FZ8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> qntvQfJssHg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/5/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> K5O4LMxdaNU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GRCOItCbUQI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/4/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> uc9_8k7WGqM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Z8TL73MJymg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gSc4LJsZ3VE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> skKe784s0sk</t>
+  </si>
+  <si>
+    <t>gV2m1xgLzXQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/3/2016</t>
+  </si>
+  <si>
+    <t>GW55Ej9vl2c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/2/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RHy6N5MnuK0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3B_0VYnrVeU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 78gWD7_A4r4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LfqqVoxHIkk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/1/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oprakdo83FE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -mZ9xHBZ9NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n7DBJNUMp5c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/31/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ahB5SnDNxgg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5LzUwcoljnE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lt7S6-WRzdE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/30/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 51EW3bcqH1s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> m2RRQBR6wOs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> blMchQA5xJ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/29/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jXOcVReBF3o</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> uM9uAlbr7No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Y_FfKjDlOJo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NO Pelicans </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/28/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> S3GAN8j8eEU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sKPmOZgGqso</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/27/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8d_zOxpeI9Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minesota Timberwolves </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JNtUTkYdeyI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/26/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JqWJGXxnoQ0</t>
+  </si>
+  <si>
+    <t>aJoTCgs2RQ8</t>
+  </si>
+  <si>
+    <t>j6OxmCbPr3E</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>yYMnDFLhSsY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">potentially have only half of the regular season games </t>
+  </si>
+  <si>
+    <t>Teams</t>
+  </si>
+  <si>
+    <t>Sacramento Kings</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Lakers</t>
+  </si>
+  <si>
+    <t>Clippers</t>
+  </si>
+  <si>
+    <t>Total games we have</t>
+  </si>
+  <si>
+    <t>Total games we need</t>
+  </si>
+  <si>
+    <t>need 1230 total games played</t>
+  </si>
+  <si>
+    <t>dbch9g8uoBA</t>
   </si>
 </sst>
 </file>
@@ -2201,21 +2600,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D412"/>
+  <dimension ref="A1:F507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
-      <selection activeCell="A409" sqref="A409:D412"/>
+    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
+      <selection activeCell="B401" sqref="B401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2228,8 +2628,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2242,8 +2645,15 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(A2:B504, "*" &amp; E2 &amp; "*")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -2256,8 +2666,15 @@
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3">
+        <f>COUNTIF(A2:B504,"*"&amp;E3&amp;"*")</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -2270,8 +2687,15 @@
       <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <f>COUNTIF(A2:B504,"*" &amp; E4 &amp; "*")</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -2284,8 +2708,15 @@
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5">
+        <f>COUNTIF(A2:B504,"*" &amp; E5 &amp; "*")</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2298,8 +2729,15 @@
       <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <f>COUNTIF(A2:B504,"*" &amp; E6 &amp; "*")</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -2312,8 +2750,15 @@
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <f>COUNTIF(A2:B504,"*" &amp; E7 &amp; "*")</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -2326,8 +2771,15 @@
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="F8">
+        <f>COUNTIF(A2:B504,"*" &amp; E8 &amp; "*")</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -2340,8 +2792,15 @@
       <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9">
+        <f>COUNTIF(A2:B504,"*" &amp; E9 &amp; "*")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -2354,8 +2813,15 @@
       <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <f>COUNTIF(A2:B504,"*" &amp; E10 &amp; "*")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -2368,8 +2834,15 @@
       <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <f>COUNTIF(A2:B504,"*" &amp; E11 &amp; "*")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -2382,8 +2855,15 @@
       <c r="D12" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <f>COUNTIF(A2:B504,"*" &amp; E12 &amp; "*")</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -2396,8 +2876,15 @@
       <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13">
+        <f>COUNTIF(A2:B504,"*" &amp; E13 &amp; "*")</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2410,8 +2897,15 @@
       <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14">
+        <f>COUNTIF(A2:B504,"*" &amp; E14 &amp; "*")</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -2424,8 +2918,15 @@
       <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="F15">
+        <f>COUNTIF(A2:B504,"*" &amp; E15 &amp; "*")</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -2438,8 +2939,15 @@
       <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16">
+        <f>COUNTIF(A2:B504,"*" &amp; E16 &amp; "*")</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -2452,8 +2960,15 @@
       <c r="D17" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17">
+        <f>COUNTIF(A2:B504,"*" &amp; E17 &amp; "*")</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -2466,8 +2981,15 @@
       <c r="D18" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <f>COUNTIF(A2:B504,"*" &amp; E18 &amp; "*")</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -2480,8 +3002,15 @@
       <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <f>COUNTIF(A2:B504,"*" &amp;E19  &amp; "*")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>54</v>
       </c>
@@ -2494,8 +3023,15 @@
       <c r="D20" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F20">
+        <f>COUNTIF(A2:B504,"*" &amp; E20 &amp; "*")</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -2508,8 +3044,15 @@
       <c r="D21" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <f>COUNTIF(A2:B504,"*" &amp; E21 &amp; "*")</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -2522,8 +3065,15 @@
       <c r="D22" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22">
+        <f>COUNTIF(A2:B504,"*" &amp; E22 &amp; "*")</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -2536,8 +3086,15 @@
       <c r="D23" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23">
+        <f>COUNTIF(A2:B504,"*" &amp; E23 &amp; "*")</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -2550,8 +3107,15 @@
       <c r="D24" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <f>COUNTIF(A2:B504,"*" &amp; E24 &amp; "*")</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
@@ -2564,8 +3128,15 @@
       <c r="D25" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="F25">
+        <f>COUNTIF(A2:B504,"*" &amp; E25 &amp; "*")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -2578,8 +3149,15 @@
       <c r="D26" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <f>COUNTIF(A2:B504,"*" &amp; E26 &amp; "*")</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>74</v>
       </c>
@@ -2592,8 +3170,15 @@
       <c r="D27" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="F27">
+        <f>COUNTIF(A2:B504,"*" &amp; E27  &amp; "*")</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -2606,8 +3191,15 @@
       <c r="D28" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F28">
+        <f>COUNTIF(A2:B504,"*" &amp; E28 &amp; "*")</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -2620,8 +3212,15 @@
       <c r="D29" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <f>COUNTIF(A2:B504,"*" &amp; E29 &amp; "*")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
@@ -2634,8 +3233,15 @@
       <c r="D30" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30">
+        <f>COUNTIF(A2:B504,"*" &amp; E30 &amp; "*")</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -2648,8 +3254,15 @@
       <c r="D31" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="F31">
+        <f>SUM(F2:F30)</f>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
@@ -2661,6 +3274,12 @@
       </c>
       <c r="D32" s="1" t="s">
         <v>87</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="F32">
+        <v>2460</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -7845,145 +8464,1446 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>74</v>
+        <v>514</v>
       </c>
       <c r="B403" t="s">
-        <v>43</v>
-      </c>
-      <c r="C403" t="s">
-        <v>606</v>
+        <v>13</v>
+      </c>
+      <c r="C403" s="5">
+        <v>42703</v>
       </c>
       <c r="D403" t="s">
-        <v>604</v>
+        <v>748</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="B404" t="s">
-        <v>72</v>
-      </c>
-      <c r="C404" s="5">
-        <v>42702</v>
+        <v>43</v>
+      </c>
+      <c r="C404" t="s">
+        <v>606</v>
       </c>
       <c r="D404" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="B405" t="s">
-        <v>192</v>
-      </c>
-      <c r="C405" t="s">
-        <v>606</v>
+        <v>72</v>
+      </c>
+      <c r="C405" s="5">
+        <v>42702</v>
       </c>
       <c r="D405" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B406" t="s">
-        <v>414</v>
+        <v>192</v>
       </c>
       <c r="C406" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D406" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="B407" t="s">
-        <v>39</v>
-      </c>
-      <c r="C407" s="5">
-        <v>42701</v>
+        <v>414</v>
+      </c>
+      <c r="C407" t="s">
+        <v>608</v>
       </c>
       <c r="D407" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="B408" t="s">
-        <v>52</v>
-      </c>
-      <c r="C408" t="s">
-        <v>608</v>
+        <v>39</v>
+      </c>
+      <c r="C408" s="5">
+        <v>42701</v>
       </c>
       <c r="D408" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B409" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C409" t="s">
         <v>608</v>
       </c>
       <c r="D409" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B410" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="C410" t="s">
         <v>608</v>
       </c>
       <c r="D410" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
       <c r="B411" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C411" t="s">
         <v>608</v>
       </c>
       <c r="D411" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="B412" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C412" t="s">
         <v>608</v>
       </c>
       <c r="D412" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A413" t="s">
+        <v>69</v>
+      </c>
+      <c r="B413" t="s">
+        <v>49</v>
+      </c>
+      <c r="C413" t="s">
+        <v>608</v>
+      </c>
+      <c r="D413" t="s">
         <v>615</v>
       </c>
     </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A414" t="s">
+        <v>69</v>
+      </c>
+      <c r="B414" t="s">
+        <v>54</v>
+      </c>
+      <c r="C414" t="s">
+        <v>616</v>
+      </c>
+      <c r="D414" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A415" t="s">
+        <v>618</v>
+      </c>
+      <c r="B415" t="s">
+        <v>91</v>
+      </c>
+      <c r="C415" s="5">
+        <v>42697</v>
+      </c>
+      <c r="D415" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A416" t="s">
+        <v>16</v>
+      </c>
+      <c r="B416" t="s">
+        <v>22</v>
+      </c>
+      <c r="C416" s="5">
+        <v>42697</v>
+      </c>
+      <c r="D416" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A417" t="s">
+        <v>54</v>
+      </c>
+      <c r="B417" t="s">
+        <v>13</v>
+      </c>
+      <c r="C417" s="5">
+        <v>42697</v>
+      </c>
+      <c r="D417" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A418" t="s">
+        <v>39</v>
+      </c>
+      <c r="B418" t="s">
+        <v>75</v>
+      </c>
+      <c r="C418" s="5">
+        <v>42697</v>
+      </c>
+      <c r="D418" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A419" t="s">
+        <v>54</v>
+      </c>
+      <c r="B419" t="s">
+        <v>111</v>
+      </c>
+      <c r="C419" t="s">
+        <v>623</v>
+      </c>
+      <c r="D419" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A420" t="s">
+        <v>114</v>
+      </c>
+      <c r="B420" t="s">
+        <v>94</v>
+      </c>
+      <c r="C420" t="s">
+        <v>623</v>
+      </c>
+      <c r="D420" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A421" t="s">
+        <v>91</v>
+      </c>
+      <c r="B421" t="s">
+        <v>86</v>
+      </c>
+      <c r="C421" t="s">
+        <v>623</v>
+      </c>
+      <c r="D421" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A422" t="s">
+        <v>57</v>
+      </c>
+      <c r="B422" t="s">
+        <v>414</v>
+      </c>
+      <c r="C422" t="s">
+        <v>627</v>
+      </c>
+      <c r="D422" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A423" t="s">
+        <v>629</v>
+      </c>
+      <c r="B423" t="s">
+        <v>105</v>
+      </c>
+      <c r="C423" t="s">
+        <v>627</v>
+      </c>
+      <c r="D423" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A424" t="s">
+        <v>91</v>
+      </c>
+      <c r="B424" t="s">
+        <v>124</v>
+      </c>
+      <c r="C424" t="s">
+        <v>631</v>
+      </c>
+      <c r="D424" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A425" t="s">
+        <v>54</v>
+      </c>
+      <c r="B425" t="s">
+        <v>94</v>
+      </c>
+      <c r="C425" t="s">
+        <v>631</v>
+      </c>
+      <c r="D425" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
+        <v>69</v>
+      </c>
+      <c r="B426" t="s">
+        <v>414</v>
+      </c>
+      <c r="C426" t="s">
+        <v>634</v>
+      </c>
+      <c r="D426" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A427" t="s">
+        <v>91</v>
+      </c>
+      <c r="B427" t="s">
+        <v>98</v>
+      </c>
+      <c r="C427" t="s">
+        <v>634</v>
+      </c>
+      <c r="D427" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
+        <v>64</v>
+      </c>
+      <c r="B428" t="s">
+        <v>75</v>
+      </c>
+      <c r="C428" t="s">
+        <v>634</v>
+      </c>
+      <c r="D428" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A429" t="s">
+        <v>57</v>
+      </c>
+      <c r="B429" t="s">
+        <v>61</v>
+      </c>
+      <c r="C429" t="s">
+        <v>638</v>
+      </c>
+      <c r="D429" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A430" t="s">
+        <v>110</v>
+      </c>
+      <c r="B430" t="s">
+        <v>65</v>
+      </c>
+      <c r="C430" t="s">
+        <v>638</v>
+      </c>
+      <c r="D430" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
+        <v>85</v>
+      </c>
+      <c r="B431" t="s">
+        <v>192</v>
+      </c>
+      <c r="C431" t="s">
+        <v>638</v>
+      </c>
+      <c r="D431" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A432" t="s">
+        <v>123</v>
+      </c>
+      <c r="B432" t="s">
+        <v>98</v>
+      </c>
+      <c r="C432" t="s">
+        <v>642</v>
+      </c>
+      <c r="D432" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A433" t="s">
+        <v>114</v>
+      </c>
+      <c r="B433" t="s">
+        <v>105</v>
+      </c>
+      <c r="C433" t="s">
+        <v>642</v>
+      </c>
+      <c r="D433" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A434" t="s">
+        <v>91</v>
+      </c>
+      <c r="B434" t="s">
+        <v>72</v>
+      </c>
+      <c r="C434" t="s">
+        <v>642</v>
+      </c>
+      <c r="D434" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A435" t="s">
+        <v>35</v>
+      </c>
+      <c r="B435" t="s">
+        <v>86</v>
+      </c>
+      <c r="C435" t="s">
+        <v>642</v>
+      </c>
+      <c r="D435" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A436" t="s">
+        <v>235</v>
+      </c>
+      <c r="B436" t="s">
+        <v>414</v>
+      </c>
+      <c r="C436" t="s">
+        <v>647</v>
+      </c>
+      <c r="D436" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A437" t="s">
+        <v>57</v>
+      </c>
+      <c r="B437" t="s">
+        <v>39</v>
+      </c>
+      <c r="C437" t="s">
+        <v>647</v>
+      </c>
+      <c r="D437" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A438" t="s">
+        <v>127</v>
+      </c>
+      <c r="B438" t="s">
+        <v>111</v>
+      </c>
+      <c r="C438" t="s">
+        <v>647</v>
+      </c>
+      <c r="D438" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A439" t="s">
+        <v>74</v>
+      </c>
+      <c r="B439" t="s">
+        <v>192</v>
+      </c>
+      <c r="C439" t="s">
+        <v>647</v>
+      </c>
+      <c r="D439" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A440" t="s">
+        <v>93</v>
+      </c>
+      <c r="B440" t="s">
+        <v>75</v>
+      </c>
+      <c r="C440" t="s">
+        <v>647</v>
+      </c>
+      <c r="D440" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A441" t="s">
+        <v>235</v>
+      </c>
+      <c r="B441" t="s">
+        <v>478</v>
+      </c>
+      <c r="C441" t="s">
+        <v>653</v>
+      </c>
+      <c r="D441" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A442" t="s">
+        <v>48</v>
+      </c>
+      <c r="B442" t="s">
+        <v>46</v>
+      </c>
+      <c r="C442" t="s">
+        <v>653</v>
+      </c>
+      <c r="D442" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A443" t="s">
+        <v>54</v>
+      </c>
+      <c r="B443" t="s">
+        <v>119</v>
+      </c>
+      <c r="C443" t="s">
+        <v>653</v>
+      </c>
+      <c r="D443" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A444" t="s">
+        <v>31</v>
+      </c>
+      <c r="B444" t="s">
+        <v>94</v>
+      </c>
+      <c r="C444" t="s">
+        <v>653</v>
+      </c>
+      <c r="D444" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A445" t="s">
+        <v>183</v>
+      </c>
+      <c r="B445" t="s">
+        <v>43</v>
+      </c>
+      <c r="C445" t="s">
+        <v>658</v>
+      </c>
+      <c r="D445" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A446" t="s">
+        <v>88</v>
+      </c>
+      <c r="B446" t="s">
+        <v>111</v>
+      </c>
+      <c r="C446" t="s">
+        <v>658</v>
+      </c>
+      <c r="D446" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A447" t="s">
+        <v>127</v>
+      </c>
+      <c r="B447" t="s">
+        <v>75</v>
+      </c>
+      <c r="C447" t="s">
+        <v>658</v>
+      </c>
+      <c r="D447" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A448" t="s">
+        <v>103</v>
+      </c>
+      <c r="B448" t="s">
+        <v>124</v>
+      </c>
+      <c r="C448" t="s">
+        <v>662</v>
+      </c>
+      <c r="D448" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A449" t="s">
+        <v>69</v>
+      </c>
+      <c r="B449" t="s">
+        <v>65</v>
+      </c>
+      <c r="C449" t="s">
+        <v>662</v>
+      </c>
+      <c r="D449" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A450" t="s">
+        <v>79</v>
+      </c>
+      <c r="B450" t="s">
+        <v>133</v>
+      </c>
+      <c r="C450" t="s">
+        <v>662</v>
+      </c>
+      <c r="D450" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A451" t="s">
+        <v>54</v>
+      </c>
+      <c r="B451" t="s">
+        <v>86</v>
+      </c>
+      <c r="C451" t="s">
+        <v>662</v>
+      </c>
+      <c r="D451" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A452" t="s">
+        <v>64</v>
+      </c>
+      <c r="B452" t="s">
+        <v>46</v>
+      </c>
+      <c r="C452" t="s">
+        <v>667</v>
+      </c>
+      <c r="D452" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A453" t="s">
+        <v>35</v>
+      </c>
+      <c r="B453" t="s">
+        <v>49</v>
+      </c>
+      <c r="C453" t="s">
+        <v>667</v>
+      </c>
+      <c r="D453" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A454" t="s">
+        <v>349</v>
+      </c>
+      <c r="B454" t="s">
+        <v>356</v>
+      </c>
+      <c r="C454" t="s">
+        <v>670</v>
+      </c>
+      <c r="D454" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A455" t="s">
+        <v>91</v>
+      </c>
+      <c r="B455" t="s">
+        <v>32</v>
+      </c>
+      <c r="C455" t="s">
+        <v>670</v>
+      </c>
+      <c r="D455" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A456" t="s">
+        <v>42</v>
+      </c>
+      <c r="B456" t="s">
+        <v>124</v>
+      </c>
+      <c r="C456" t="s">
+        <v>670</v>
+      </c>
+      <c r="D456" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A457" t="s">
+        <v>57</v>
+      </c>
+      <c r="B457" t="s">
+        <v>192</v>
+      </c>
+      <c r="C457" t="s">
+        <v>670</v>
+      </c>
+      <c r="D457" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A458" t="s">
+        <v>123</v>
+      </c>
+      <c r="B458" t="s">
+        <v>43</v>
+      </c>
+      <c r="C458" s="5">
+        <v>42683</v>
+      </c>
+      <c r="D458" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A459" t="s">
+        <v>114</v>
+      </c>
+      <c r="B459" t="s">
+        <v>119</v>
+      </c>
+      <c r="C459" s="5">
+        <v>42683</v>
+      </c>
+      <c r="D459" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A460" t="s">
+        <v>72</v>
+      </c>
+      <c r="B460" t="s">
+        <v>31</v>
+      </c>
+      <c r="C460" s="5">
+        <v>42683</v>
+      </c>
+      <c r="D460" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A461" t="s">
+        <v>57</v>
+      </c>
+      <c r="B461" t="s">
+        <v>74</v>
+      </c>
+      <c r="C461" s="5">
+        <v>42683</v>
+      </c>
+      <c r="D461" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A462" t="s">
+        <v>123</v>
+      </c>
+      <c r="B462" t="s">
+        <v>414</v>
+      </c>
+      <c r="C462" t="s">
+        <v>679</v>
+      </c>
+      <c r="D462" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A463" t="s">
+        <v>183</v>
+      </c>
+      <c r="B463" t="s">
+        <v>39</v>
+      </c>
+      <c r="C463" t="s">
+        <v>679</v>
+      </c>
+      <c r="D463" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A464" t="s">
+        <v>60</v>
+      </c>
+      <c r="B464" t="s">
+        <v>58</v>
+      </c>
+      <c r="C464" t="s">
+        <v>679</v>
+      </c>
+      <c r="D464" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A465" t="s">
+        <v>74</v>
+      </c>
+      <c r="B465" t="s">
+        <v>75</v>
+      </c>
+      <c r="C465" t="s">
+        <v>679</v>
+      </c>
+      <c r="D465" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A466" t="s">
+        <v>42</v>
+      </c>
+      <c r="B466" t="s">
+        <v>43</v>
+      </c>
+      <c r="C466" t="s">
+        <v>684</v>
+      </c>
+      <c r="D466" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A467" t="s">
+        <v>108</v>
+      </c>
+      <c r="B467" t="s">
+        <v>133</v>
+      </c>
+      <c r="C467" t="s">
+        <v>684</v>
+      </c>
+      <c r="D467" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A468" t="s">
+        <v>48</v>
+      </c>
+      <c r="B468" t="s">
+        <v>105</v>
+      </c>
+      <c r="C468" t="s">
+        <v>684</v>
+      </c>
+      <c r="D468" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A469" t="s">
+        <v>51</v>
+      </c>
+      <c r="B469" t="s">
+        <v>55</v>
+      </c>
+      <c r="C469" t="s">
+        <v>684</v>
+      </c>
+      <c r="D469" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A470" t="s">
+        <v>183</v>
+      </c>
+      <c r="B470" t="s">
+        <v>414</v>
+      </c>
+      <c r="C470" t="s">
+        <v>689</v>
+      </c>
+      <c r="D470" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A471" t="s">
+        <v>85</v>
+      </c>
+      <c r="B471" t="s">
+        <v>70</v>
+      </c>
+      <c r="C471" t="s">
+        <v>689</v>
+      </c>
+      <c r="D471" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A472" t="s">
+        <v>130</v>
+      </c>
+      <c r="B472" t="s">
+        <v>72</v>
+      </c>
+      <c r="C472" t="s">
+        <v>689</v>
+      </c>
+      <c r="D472" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A473" t="s">
+        <v>45</v>
+      </c>
+      <c r="B473" t="s">
+        <v>46</v>
+      </c>
+      <c r="C473" t="s">
+        <v>693</v>
+      </c>
+      <c r="D473" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A474" t="s">
+        <v>35</v>
+      </c>
+      <c r="B474" t="s">
+        <v>83</v>
+      </c>
+      <c r="C474" t="s">
+        <v>693</v>
+      </c>
+      <c r="D474" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A475" t="s">
+        <v>91</v>
+      </c>
+      <c r="B475" t="s">
+        <v>121</v>
+      </c>
+      <c r="C475" t="s">
+        <v>696</v>
+      </c>
+      <c r="D475" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A476" t="s">
+        <v>69</v>
+      </c>
+      <c r="B476" t="s">
+        <v>61</v>
+      </c>
+      <c r="C476" t="s">
+        <v>696</v>
+      </c>
+      <c r="D476" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A477" t="s">
+        <v>177</v>
+      </c>
+      <c r="B477" t="s">
+        <v>133</v>
+      </c>
+      <c r="C477" t="s">
+        <v>696</v>
+      </c>
+      <c r="D477" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A478" t="s">
+        <v>93</v>
+      </c>
+      <c r="B478" t="s">
+        <v>192</v>
+      </c>
+      <c r="C478" t="s">
+        <v>696</v>
+      </c>
+      <c r="D478" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A479" t="s">
+        <v>51</v>
+      </c>
+      <c r="B479" t="s">
+        <v>124</v>
+      </c>
+      <c r="C479" t="s">
+        <v>702</v>
+      </c>
+      <c r="D479" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A480" t="s">
+        <v>54</v>
+      </c>
+      <c r="B480" t="s">
+        <v>75</v>
+      </c>
+      <c r="C480" t="s">
+        <v>702</v>
+      </c>
+      <c r="D480" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A481" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B481" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C481" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="D481" s="3" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A482" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B482" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C482" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="D482" s="3" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A483" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B483" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C483" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="D483" s="3" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A484" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B484" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C484" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="D484" s="3" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A485" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B485" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C485" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="D485" s="3" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A486" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B486" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C486" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="D486" s="3" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A487" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B487" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C487" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="D487" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A488" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B488" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C488" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="D488" s="3" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A489" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B489" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C489" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="D489" s="3" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A490" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B490" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C490" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="D490" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A491" t="s">
+        <v>123</v>
+      </c>
+      <c r="B491" t="s">
+        <v>65</v>
+      </c>
+      <c r="C491" t="s">
+        <v>717</v>
+      </c>
+      <c r="D491" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A492" t="s">
+        <v>88</v>
+      </c>
+      <c r="B492" t="s">
+        <v>105</v>
+      </c>
+      <c r="C492" t="s">
+        <v>717</v>
+      </c>
+      <c r="D492" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A493" t="s">
+        <v>91</v>
+      </c>
+      <c r="B493" t="s">
+        <v>67</v>
+      </c>
+      <c r="C493" t="s">
+        <v>717</v>
+      </c>
+      <c r="D493" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A494" t="s">
+        <v>60</v>
+      </c>
+      <c r="B494" t="s">
+        <v>356</v>
+      </c>
+      <c r="C494" t="s">
+        <v>721</v>
+      </c>
+      <c r="D494" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A495" t="s">
+        <v>235</v>
+      </c>
+      <c r="B495" t="s">
+        <v>124</v>
+      </c>
+      <c r="C495" t="s">
+        <v>721</v>
+      </c>
+      <c r="D495" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A496" t="s">
+        <v>51</v>
+      </c>
+      <c r="B496" t="s">
+        <v>133</v>
+      </c>
+      <c r="C496" t="s">
+        <v>721</v>
+      </c>
+      <c r="D496" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A497" t="s">
+        <v>91</v>
+      </c>
+      <c r="B497" t="s">
+        <v>725</v>
+      </c>
+      <c r="C497" t="s">
+        <v>726</v>
+      </c>
+      <c r="D497" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A498" t="s">
+        <v>35</v>
+      </c>
+      <c r="B498" t="s">
+        <v>72</v>
+      </c>
+      <c r="C498" t="s">
+        <v>726</v>
+      </c>
+      <c r="D498" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A499" t="s">
+        <v>54</v>
+      </c>
+      <c r="B499" t="s">
+        <v>133</v>
+      </c>
+      <c r="C499" t="s">
+        <v>729</v>
+      </c>
+      <c r="D499" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A500" t="s">
+        <v>731</v>
+      </c>
+      <c r="B500" t="s">
+        <v>221</v>
+      </c>
+      <c r="C500" s="5">
+        <v>42669</v>
+      </c>
+      <c r="D500" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A501" t="s">
+        <v>235</v>
+      </c>
+      <c r="B501" t="s">
+        <v>98</v>
+      </c>
+      <c r="C501" t="s">
+        <v>733</v>
+      </c>
+      <c r="D501" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A502" t="s">
+        <v>8</v>
+      </c>
+      <c r="B502" t="s">
+        <v>25</v>
+      </c>
+      <c r="C502" s="5">
+        <v>42668</v>
+      </c>
+      <c r="D502" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A503" t="s">
+        <v>7</v>
+      </c>
+      <c r="B503" t="s">
+        <v>11</v>
+      </c>
+      <c r="C503" s="5">
+        <v>42668</v>
+      </c>
+      <c r="D503" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A504" t="s">
+        <v>737</v>
+      </c>
+      <c r="B504" t="s">
+        <v>17</v>
+      </c>
+      <c r="C504" s="5">
+        <v>42668</v>
+      </c>
+      <c r="D504" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A506" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A507" t="s">
+        <v>747</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="E2:E30">
+    <sortCondition ref="E2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>